<commit_message>
updating pins for sd, eeprom, flash, rj45.
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="0" windowWidth="11080" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="14160" windowWidth="8280" windowHeight="14160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="432">
   <si>
     <t>QTY</t>
   </si>
@@ -1302,6 +1302,24 @@
   </si>
   <si>
     <t>Ethernet Port</t>
+  </si>
+  <si>
+    <t>MT25Q</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Alt</t>
+  </si>
+  <si>
+    <t>On pin list?</t>
+  </si>
+  <si>
+    <t>On schematic?</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -1409,7 +1427,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1499,8 +1517,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1600,8 +1620,9 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1646,6 +1667,7 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1690,6 +1712,7 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2019,10 +2042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2031,143 +2054,192 @@
     <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" s="14" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="B1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D1" t="s">
+        <v>429</v>
+      </c>
+      <c r="E1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>415</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B3" s="32" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>416</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B4" s="30" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>426</v>
+      </c>
+      <c r="D4" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>417</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B5" s="31" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>418</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B6" s="31" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>419</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B7" s="29" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="D7" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
         <v>420</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="D8" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
         <v>425</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B10" s="33" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="14" t="s">
+      <c r="D10" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="14" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" s="34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
         <v>415</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B14" s="32" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
         <v>416</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B15" s="30" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="C15" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
         <v>417</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B16" s="31" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>418</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>419</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>420</v>
-      </c>
-      <c r="B17" t="s">
-        <v>422</v>
+        <v>418</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>423</v>
+        <v>419</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>422</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>424</v>
+      </c>
+      <c r="B21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>425</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B22" s="33" t="s">
         <v>343</v>
       </c>
     </row>

</xml_diff>